<commit_message>
added sku mapping excel file
</commit_message>
<xml_diff>
--- a/public/uploads/excel-formats/customers-po.xlsx
+++ b/public/uploads/excel-formats/customers-po.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>HSN</t>
   </si>
@@ -443,7 +443,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,51 +513,21 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>